<commit_message>
added justification and some components
</commit_message>
<xml_diff>
--- a/lab2/embedded_justification_spreadsheet.xlsx
+++ b/lab2/embedded_justification_spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\embedded_team_repo\Embedded\lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{578E13FC-A9F0-4542-A8CD-FFFB40391E96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7F376A-80C9-426C-AE73-A399DD47DCEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1553E207-5CAF-4B1A-ABF7-752273BD112F}"/>
+    <workbookView xWindow="5760" yWindow="2952" windowWidth="17280" windowHeight="8964" xr2:uid="{1553E207-5CAF-4B1A-ABF7-752273BD112F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="100">
   <si>
     <t xml:space="preserve">Component </t>
   </si>
@@ -223,13 +223,121 @@
   </si>
   <si>
     <t>Power LED</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>Microchip</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>Kingbright</t>
+  </si>
+  <si>
+    <t>Alpha (Taiwan)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Rotary Encoder</t>
+  </si>
+  <si>
+    <t>Contains SW3 and Encoder</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>Adjustable resistor</t>
+  </si>
+  <si>
+    <t>ALPS</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>External Pullup resistor</t>
+  </si>
+  <si>
+    <t>Current limiter</t>
+  </si>
+  <si>
+    <t>Power indicator</t>
+  </si>
+  <si>
+    <t>Smooths VPOT output</t>
+  </si>
+  <si>
+    <t>LED voltage regulator</t>
+  </si>
+  <si>
+    <t>Smooths voltage regulator output</t>
+  </si>
+  <si>
+    <t>Smooths voltage regulator input</t>
+  </si>
+  <si>
+    <t>3.3V rail noise reduction</t>
+  </si>
+  <si>
+    <t>Reccomended by PIC</t>
+  </si>
+  <si>
+    <t>Voltage smoothing on VREF</t>
+  </si>
+  <si>
+    <t>Voltage smoothing</t>
+  </si>
+  <si>
+    <t>Main MCU</t>
+  </si>
+  <si>
+    <t>Steps down USB5V to 3.3V rail</t>
+  </si>
+  <si>
+    <t>User input</t>
+  </si>
+  <si>
+    <t>MCU reset</t>
+  </si>
+  <si>
+    <t>MCU output</t>
+  </si>
+  <si>
+    <t>User resistance input</t>
+  </si>
+  <si>
+    <t>User rotation input</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +347,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -264,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -272,6 +388,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,26 +703,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3707CC55-1DFD-425B-9579-60E26BD568A1}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C35"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -615,8 +744,14 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -626,8 +761,14 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -637,8 +778,14 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -648,8 +795,14 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -659,8 +812,14 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -670,8 +829,14 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -681,8 +846,14 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -692,8 +863,14 @@
       <c r="C10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -703,8 +880,14 @@
       <c r="C11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -714,8 +897,14 @@
       <c r="C12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -725,8 +914,14 @@
       <c r="C13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -736,8 +931,14 @@
       <c r="C14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -747,8 +948,14 @@
       <c r="C15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -758,8 +965,14 @@
       <c r="C16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -769,8 +982,14 @@
       <c r="C17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
@@ -780,8 +999,14 @@
       <c r="C18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -791,8 +1016,14 @@
       <c r="C19" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -802,8 +1033,14 @@
       <c r="C20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -813,8 +1050,14 @@
       <c r="C21" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
@@ -824,8 +1067,14 @@
       <c r="C22" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -835,8 +1084,14 @@
       <c r="C23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -846,8 +1101,14 @@
       <c r="C24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
@@ -857,8 +1118,14 @@
       <c r="C26" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -868,8 +1135,14 @@
       <c r="C27" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
@@ -879,8 +1152,14 @@
       <c r="C28" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
@@ -890,8 +1169,14 @@
       <c r="C29" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
@@ -901,8 +1186,14 @@
       <c r="C30" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
@@ -912,8 +1203,14 @@
       <c r="C31" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>56</v>
       </c>
@@ -923,8 +1220,14 @@
       <c r="C32" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>59</v>
       </c>
@@ -934,8 +1237,14 @@
       <c r="C33" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>61</v>
       </c>
@@ -945,8 +1254,14 @@
       <c r="C34" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
@@ -956,8 +1271,49 @@
       <c r="C35" t="s">
         <v>62</v>
       </c>
+      <c r="D35" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>